<commit_message>
Add directory “Topcoder”, and update some leetcode solutions.
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -1285,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1449,7 +1449,7 @@
         <v>0.35599999999999998</v>
       </c>
       <c r="E10" s="20"/>
-      <c r="F10" s="8"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7">
@@ -1479,7 +1479,7 @@
         <v>0.309</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7">
@@ -1599,7 +1599,7 @@
         <v>0.25800000000000001</v>
       </c>
       <c r="E20" s="21"/>
-      <c r="F20" s="8"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7">
@@ -1854,7 +1854,7 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="E37" s="20"/>
-      <c r="F37" s="8"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7">
@@ -2439,7 +2439,7 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="E76" s="20"/>
-      <c r="F76" s="8"/>
+      <c r="F76" s="19"/>
       <c r="G76" s="9"/>
     </row>
     <row r="77" spans="1:7">
@@ -2709,7 +2709,7 @@
         <v>0.221</v>
       </c>
       <c r="E94" s="21"/>
-      <c r="F94" s="8"/>
+      <c r="F94" s="19"/>
       <c r="G94" s="9"/>
     </row>
     <row r="95" spans="1:7">
@@ -2724,7 +2724,7 @@
         <v>0.222</v>
       </c>
       <c r="E95" s="21"/>
-      <c r="F95" s="8"/>
+      <c r="F95" s="19"/>
       <c r="G95" s="9"/>
     </row>
     <row r="96" spans="1:7">
@@ -2754,7 +2754,7 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="E97" s="22"/>
-      <c r="F97" s="8"/>
+      <c r="F97" s="19"/>
       <c r="G97" s="9"/>
     </row>
     <row r="98" spans="1:7">
@@ -2949,7 +2949,7 @@
         <v>0.247</v>
       </c>
       <c r="E110" s="21"/>
-      <c r="F110" s="8"/>
+      <c r="F110" s="19"/>
       <c r="G110" s="9"/>
     </row>
     <row r="111" spans="1:7">
@@ -3054,7 +3054,7 @@
         <v>0.27400000000000002</v>
       </c>
       <c r="E117" s="21"/>
-      <c r="F117" s="8"/>
+      <c r="F117" s="19"/>
       <c r="G117" s="9"/>
     </row>
     <row r="118" spans="1:7">
@@ -3279,7 +3279,7 @@
         <v>0.215</v>
       </c>
       <c r="E132" s="20"/>
-      <c r="F132" s="8"/>
+      <c r="F132" s="21"/>
       <c r="G132" s="9"/>
     </row>
     <row r="133" spans="1:7">
@@ -3294,7 +3294,7 @@
         <v>0.314</v>
       </c>
       <c r="E133" s="20"/>
-      <c r="F133" s="8"/>
+      <c r="F133" s="21"/>
       <c r="G133" s="9"/>
     </row>
     <row r="134" spans="1:7">
@@ -3579,7 +3579,7 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="E152" s="21"/>
-      <c r="F152" s="8"/>
+      <c r="F152" s="19"/>
       <c r="G152" s="9"/>
     </row>
     <row r="153" spans="1:7">

</xml_diff>